<commit_message>
add Book Value, Increasing sales revenues, Increasing net profit
</commit_message>
<xml_diff>
--- a/Livechat.xlsx
+++ b/Livechat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30041519\Analizy giełdowe\Analiza wybranej spółki\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30041519\Analizy giełdowe\Analiza wybranej spółki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A2C290-28B6-4AD9-8F8E-FD54374EBC59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A403821-EF4C-4299-A927-FF797C7D574A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>LVC (LIVECHAT)</t>
   </si>
   <si>
-    <t>w tys. PLN</t>
-  </si>
-  <si>
     <t>Przychody ze sprzedaży</t>
   </si>
   <si>
@@ -228,13 +225,22 @@
   </si>
   <si>
     <t>Temp7</t>
+  </si>
+  <si>
+    <t>Stopa dywidendy</t>
+  </si>
+  <si>
+    <t>Wartość dywidendy na akcje</t>
+  </si>
+  <si>
+    <t>Lata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +250,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,17 +279,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -554,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO13"/>
+  <dimension ref="A1:BQ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BN4" sqref="BN4"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,210 +582,216 @@
     <col min="2" max="67" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BM1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BF1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BM1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="1" t="s">
-        <v>55</v>
+      <c r="BQ1" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,7 +904,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1092,7 @@
         <v>1611</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1280,7 @@
         <v>-321</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1445,8 +1467,14 @@
       <c r="BO5">
         <v>6872</v>
       </c>
+      <c r="BP5" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="BQ5">
+        <v>0.37</v>
+      </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1633,8 +1661,14 @@
       <c r="BO6">
         <v>6736</v>
       </c>
+      <c r="BP6" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="BQ6">
+        <v>0.71</v>
+      </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1821,8 +1855,14 @@
       <c r="BO7">
         <v>8052</v>
       </c>
+      <c r="BP7" s="2">
+        <v>2.3E-2</v>
+      </c>
+      <c r="BQ7">
+        <v>1.08</v>
+      </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2009,8 +2049,14 @@
       <c r="BO8">
         <v>11536</v>
       </c>
+      <c r="BP8" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="BQ8">
+        <v>1.41</v>
+      </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2197,8 +2243,14 @@
       <c r="BO9">
         <v>-4616</v>
       </c>
+      <c r="BP9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="BQ9">
+        <v>1.77</v>
+      </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2385,8 +2437,14 @@
       <c r="BO10">
         <v>2490</v>
       </c>
+      <c r="BP10" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="BQ10">
+        <v>1.95</v>
+      </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2503,7 @@
         <v>62095</v>
       </c>
       <c r="U11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V11">
         <v>26823</v>
@@ -2547,7 +2605,7 @@
         <v>73755</v>
       </c>
       <c r="BE11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BF11">
         <v>66231</v>
@@ -2573,11 +2631,17 @@
       <c r="BO11">
         <v>4959</v>
       </c>
+      <c r="BP11" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="BQ11">
+        <v>2.48</v>
+      </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
   </sheetData>

</xml_diff>